<commit_message>
Added all the single-phase non-aqueous liquids from Melinder 2010
Moved the enum of property indices to CoolProp.h
</commit_message>
<xml_diff>
--- a/Docs/Melinder coefficients.xlsx
+++ b/Docs/Melinder coefficients.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="37">
   <si>
     <t>Tf</t>
   </si>
@@ -101,6 +104,33 @@
   <si>
     <t>d-Limonene, extract from orange/lemon peel oils</t>
   </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>DEB</t>
+  </si>
+  <si>
+    <t>TCO</t>
+  </si>
+  <si>
+    <t>HCB</t>
+  </si>
+  <si>
+    <t>SAB</t>
+  </si>
+  <si>
+    <t>PMS2</t>
+  </si>
+  <si>
+    <t>PMS1</t>
+  </si>
+  <si>
+    <t>HFE</t>
+  </si>
+  <si>
+    <t>HCM</t>
+  </si>
 </sst>
 </file>
 
@@ -149,6 +179,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sample calcs"/>
+      <sheetName val="Water saturation table"/>
+      <sheetName val="Sheet3"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="Props"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -438,30 +488,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:L129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -480,8 +530,23 @@
       <c r="F5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -500,8 +565,23 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-81</v>
       </c>
@@ -520,8 +600,31 @@
       <c r="F7">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7">
+        <f>B7+273.15</f>
+        <v>373.15</v>
+      </c>
+      <c r="I7">
+        <f>[1]!Props("D","T",B7+273.15,"P",101.325,G7)</f>
+        <v>803.65943670000001</v>
+      </c>
+      <c r="J7">
+        <f>[1]!Props("C","T",H7,"P",101.325,G7)*1000</f>
+        <v>2072.8188439999999</v>
+      </c>
+      <c r="K7">
+        <f>[1]!Props("L","T",H7,"P",101.325,G7)*1000</f>
+        <v>0.1121272734</v>
+      </c>
+      <c r="L7">
+        <f>[1]!Props("V","T",H7,"P",101.325,G7)*1000</f>
+        <v>0.41322388654426123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>80</v>
       </c>
@@ -537,8 +640,31 @@
       <c r="F8">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ref="H8:H16" si="0">B8+273.15</f>
+        <v>353.15</v>
+      </c>
+      <c r="I8">
+        <f>[1]!Props("D","T",B8+273.15,"P",101.325,G8)</f>
+        <v>818.28307670000004</v>
+      </c>
+      <c r="J8">
+        <f>[1]!Props("C","T",H8,"P",101.325,G8)*1000</f>
+        <v>2015.3036439999998</v>
+      </c>
+      <c r="K8">
+        <f>[1]!Props("L","T",H8,"P",101.325,G8)*1000</f>
+        <v>0.1162545534</v>
+      </c>
+      <c r="L8">
+        <f>[1]!Props("V","T",H8,"P",101.325,G8)*1000</f>
+        <v>0.46179586077983192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>60</v>
       </c>
@@ -554,8 +680,31 @@
       <c r="F9">
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>333.15</v>
+      </c>
+      <c r="I9">
+        <f>[1]!Props("D","T",B9+273.15,"P",101.325,G9)</f>
+        <v>832.90671670000006</v>
+      </c>
+      <c r="J9">
+        <f>[1]!Props("C","T",H9,"P",101.325,G9)*1000</f>
+        <v>1957.788444</v>
+      </c>
+      <c r="K9">
+        <f>[1]!Props("L","T",H9,"P",101.325,G9)*1000</f>
+        <v>0.12038183340000001</v>
+      </c>
+      <c r="L9">
+        <f>[1]!Props("V","T",H9,"P",101.325,G9)*1000</f>
+        <v>0.54594749223299666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>40</v>
       </c>
@@ -571,8 +720,31 @@
       <c r="F10">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>313.14999999999998</v>
+      </c>
+      <c r="I10">
+        <f>[1]!Props("D","T",B10+273.15,"P",101.325,G10)</f>
+        <v>847.53035669999997</v>
+      </c>
+      <c r="J10">
+        <f>[1]!Props("C","T",H10,"P",101.325,G10)*1000</f>
+        <v>1900.273244</v>
+      </c>
+      <c r="K10">
+        <f>[1]!Props("L","T",H10,"P",101.325,G10)*1000</f>
+        <v>0.1245091134</v>
+      </c>
+      <c r="L10">
+        <f>[1]!Props("V","T",H10,"P",101.325,G10)*1000</f>
+        <v>0.68279123394809482</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>20</v>
       </c>
@@ -588,8 +760,31 @@
       <c r="F11">
         <v>0.91</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>293.14999999999998</v>
+      </c>
+      <c r="I11">
+        <f>[1]!Props("D","T",B11+273.15,"P",101.325,G11)</f>
+        <v>862.15399669999999</v>
+      </c>
+      <c r="J11">
+        <f>[1]!Props("C","T",H11,"P",101.325,G11)*1000</f>
+        <v>1842.7580439999999</v>
+      </c>
+      <c r="K11">
+        <f>[1]!Props("L","T",H11,"P",101.325,G11)*1000</f>
+        <v>0.12863639339999999</v>
+      </c>
+      <c r="L11">
+        <f>[1]!Props("V","T",H11,"P",101.325,G11)*1000</f>
+        <v>0.90336075591742049</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0</v>
       </c>
@@ -605,8 +800,31 @@
       <c r="F12">
         <v>1.23</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="I12">
+        <f>[1]!Props("D","T",B12+273.15,"P",101.325,G12)</f>
+        <v>876.77763670000002</v>
+      </c>
+      <c r="J12">
+        <f>[1]!Props("C","T",H12,"P",101.325,G12)*1000</f>
+        <v>1785.2428439999999</v>
+      </c>
+      <c r="K12">
+        <f>[1]!Props("L","T",H12,"P",101.325,G12)*1000</f>
+        <v>0.1327636734</v>
+      </c>
+      <c r="L12">
+        <f>[1]!Props("V","T",H12,"P",101.325,G12)*1000</f>
+        <v>1.2643599329463697</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>-20</v>
       </c>
@@ -622,8 +840,31 @@
       <c r="F13">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>253.14999999999998</v>
+      </c>
+      <c r="I13">
+        <f>[1]!Props("D","T",B13+273.15,"P",101.325,G13)</f>
+        <v>891.40127670000004</v>
+      </c>
+      <c r="J13">
+        <f>[1]!Props("C","T",H13,"P",101.325,G13)*1000</f>
+        <v>1727.7276440000001</v>
+      </c>
+      <c r="K13">
+        <f>[1]!Props("L","T",H13,"P",101.325,G13)*1000</f>
+        <v>0.13689095340000001</v>
+      </c>
+      <c r="L13">
+        <f>[1]!Props("V","T",H13,"P",101.325,G13)*1000</f>
+        <v>1.8720457215590462</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>-40</v>
       </c>
@@ -639,8 +880,31 @@
       <c r="F14">
         <v>2.88</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>233.14999999999998</v>
+      </c>
+      <c r="I14">
+        <f>[1]!Props("D","T",B14+273.15,"P",101.325,G14)</f>
+        <v>906.02491670000006</v>
+      </c>
+      <c r="J14">
+        <f>[1]!Props("C","T",H14,"P",101.325,G14)*1000</f>
+        <v>1670.212444</v>
+      </c>
+      <c r="K14">
+        <f>[1]!Props("L","T",H14,"P",101.325,G14)*1000</f>
+        <v>0.1410182334</v>
+      </c>
+      <c r="L14">
+        <f>[1]!Props("V","T",H14,"P",101.325,G14)*1000</f>
+        <v>2.9322324788247176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>-60</v>
       </c>
@@ -656,8 +920,31 @@
       <c r="F15">
         <v>5.12</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>213.14999999999998</v>
+      </c>
+      <c r="I15">
+        <f>[1]!Props("D","T",B15+273.15,"P",101.325,G15)</f>
+        <v>920.64855669999997</v>
+      </c>
+      <c r="J15">
+        <f>[1]!Props("C","T",H15,"P",101.325,G15)*1000</f>
+        <v>1612.697244</v>
+      </c>
+      <c r="K15">
+        <f>[1]!Props("L","T",H15,"P",101.325,G15)*1000</f>
+        <v>0.14514551340000001</v>
+      </c>
+      <c r="L15">
+        <f>[1]!Props("V","T",H15,"P",101.325,G15)*1000</f>
+        <v>4.8586606837927322</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>-80</v>
       </c>
@@ -673,23 +960,46 @@
       <c r="F16">
         <v>8.43</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>193.14999999999998</v>
+      </c>
+      <c r="I16">
+        <f>[1]!Props("D","T",B16+273.15,"P",101.325,G16)</f>
+        <v>935.27219669999999</v>
+      </c>
+      <c r="J16">
+        <f>[1]!Props("C","T",H16,"P",101.325,G16)*1000</f>
+        <v>1555.1820439999999</v>
+      </c>
+      <c r="K16">
+        <f>[1]!Props("L","T",H16,"P",101.325,G16)*1000</f>
+        <v>0.14927279340000002</v>
+      </c>
+      <c r="L16">
+        <f>[1]!Props("V","T",H16,"P",101.325,G16)*1000</f>
+        <v>8.5166924030952291</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -708,8 +1018,23 @@
       <c r="F22" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -728,8 +1053,23 @@
       <c r="F23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23" t="s">
+        <v>9</v>
+      </c>
+      <c r="L23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-81</v>
       </c>
@@ -748,8 +1088,31 @@
       <c r="F24">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24">
+        <f>B24+273.15</f>
+        <v>373.15</v>
+      </c>
+      <c r="I24">
+        <f>[1]!Props("D","T",B24+273.15,"P",101.325,G24)</f>
+        <v>703.5092578</v>
+      </c>
+      <c r="J24">
+        <f>[1]!Props("C","T",H24,"P",101.325,G24)*1000</f>
+        <v>2453.0905779999998</v>
+      </c>
+      <c r="K24">
+        <f>[1]!Props("L","T",H24,"P",101.325,G24)*1000</f>
+        <v>9.7291242200000003E-2</v>
+      </c>
+      <c r="L24">
+        <f>[1]!Props("V","T",H24,"P",101.325,G24)*1000</f>
+        <v>0.58903846612052146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>80</v>
       </c>
@@ -765,8 +1128,31 @@
       <c r="F25">
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25:H33" si="1">B25+273.15</f>
+        <v>353.15</v>
+      </c>
+      <c r="I25">
+        <f>[1]!Props("D","T",B25+273.15,"P",101.325,G25)</f>
+        <v>717.88501780000001</v>
+      </c>
+      <c r="J25">
+        <f>[1]!Props("C","T",H25,"P",101.325,G25)*1000</f>
+        <v>2366.8481779999997</v>
+      </c>
+      <c r="K25">
+        <f>[1]!Props("L","T",H25,"P",101.325,G25)*1000</f>
+        <v>0.10031548220000001</v>
+      </c>
+      <c r="L25">
+        <f>[1]!Props("V","T",H25,"P",101.325,G25)*1000</f>
+        <v>0.53505149415664033</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>60</v>
       </c>
@@ -782,8 +1168,31 @@
       <c r="F26">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>333.15</v>
+      </c>
+      <c r="I26">
+        <f>[1]!Props("D","T",B26+273.15,"P",101.325,G26)</f>
+        <v>732.26077780000003</v>
+      </c>
+      <c r="J26">
+        <f>[1]!Props("C","T",H26,"P",101.325,G26)*1000</f>
+        <v>2280.6057780000001</v>
+      </c>
+      <c r="K26">
+        <f>[1]!Props("L","T",H26,"P",101.325,G26)*1000</f>
+        <v>0.10333972220000001</v>
+      </c>
+      <c r="L26">
+        <f>[1]!Props("V","T",H26,"P",101.325,G26)*1000</f>
+        <v>0.57450643428405557</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>40</v>
       </c>
@@ -799,8 +1208,31 @@
       <c r="F27">
         <v>0.93</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>313.14999999999998</v>
+      </c>
+      <c r="I27">
+        <f>[1]!Props("D","T",B27+273.15,"P",101.325,G27)</f>
+        <v>746.63653780000004</v>
+      </c>
+      <c r="J27">
+        <f>[1]!Props("C","T",H27,"P",101.325,G27)*1000</f>
+        <v>2194.363378</v>
+      </c>
+      <c r="K27">
+        <f>[1]!Props("L","T",H27,"P",101.325,G27)*1000</f>
+        <v>0.10636396220000001</v>
+      </c>
+      <c r="L27">
+        <f>[1]!Props("V","T",H27,"P",101.325,G27)*1000</f>
+        <v>0.72919151086326872</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>20</v>
       </c>
@@ -816,8 +1248,31 @@
       <c r="F28">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>36</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>293.14999999999998</v>
+      </c>
+      <c r="I28">
+        <f>[1]!Props("D","T",B28+273.15,"P",101.325,G28)</f>
+        <v>761.01229780000006</v>
+      </c>
+      <c r="J28">
+        <f>[1]!Props("C","T",H28,"P",101.325,G28)*1000</f>
+        <v>2108.1209779999999</v>
+      </c>
+      <c r="K28">
+        <f>[1]!Props("L","T",H28,"P",101.325,G28)*1000</f>
+        <v>0.10938820220000001</v>
+      </c>
+      <c r="L28">
+        <f>[1]!Props("V","T",H28,"P",101.325,G28)*1000</f>
+        <v>1.0940463012941049</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>0</v>
       </c>
@@ -833,8 +1288,31 @@
       <c r="F29">
         <v>1.93</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="I29">
+        <f>[1]!Props("D","T",B29+273.15,"P",101.325,G29)</f>
+        <v>775.38805780000007</v>
+      </c>
+      <c r="J29">
+        <f>[1]!Props("C","T",H29,"P",101.325,G29)*1000</f>
+        <v>2021.8785779999998</v>
+      </c>
+      <c r="K29">
+        <f>[1]!Props("L","T",H29,"P",101.325,G29)*1000</f>
+        <v>0.11241244220000002</v>
+      </c>
+      <c r="L29">
+        <f>[1]!Props("V","T",H29,"P",101.325,G29)*1000</f>
+        <v>1.9403371178032227</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>-20</v>
       </c>
@@ -850,8 +1328,31 @@
       <c r="F30">
         <v>3.23</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>36</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>253.14999999999998</v>
+      </c>
+      <c r="I30">
+        <f>[1]!Props("D","T",B30+273.15,"P",101.325,G30)</f>
+        <v>789.76381780000008</v>
+      </c>
+      <c r="J30">
+        <f>[1]!Props("C","T",H30,"P",101.325,G30)*1000</f>
+        <v>1935.6361779999997</v>
+      </c>
+      <c r="K30">
+        <f>[1]!Props("L","T",H30,"P",101.325,G30)*1000</f>
+        <v>0.1154366822</v>
+      </c>
+      <c r="L30">
+        <f>[1]!Props("V","T",H30,"P",101.325,G30)*1000</f>
+        <v>4.0678606972066591</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>-40</v>
       </c>
@@ -867,8 +1368,31 @@
       <c r="F31">
         <v>7.06</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>233.14999999999998</v>
+      </c>
+      <c r="I31">
+        <f>[1]!Props("D","T",B31+273.15,"P",101.325,G31)</f>
+        <v>804.1395778000001</v>
+      </c>
+      <c r="J31">
+        <f>[1]!Props("C","T",H31,"P",101.325,G31)*1000</f>
+        <v>1849.3937779999999</v>
+      </c>
+      <c r="K31">
+        <f>[1]!Props("L","T",H31,"P",101.325,G31)*1000</f>
+        <v>0.11846092220000001</v>
+      </c>
+      <c r="L31">
+        <f>[1]!Props("V","T",H31,"P",101.325,G31)*1000</f>
+        <v>10.080970502738086</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>-60</v>
       </c>
@@ -884,8 +1408,31 @@
       <c r="F32">
         <v>23.9</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>36</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>213.14999999999998</v>
+      </c>
+      <c r="I32">
+        <f>[1]!Props("D","T",B32+273.15,"P",101.325,G32)</f>
+        <v>818.5153378</v>
+      </c>
+      <c r="J32">
+        <f>[1]!Props("C","T",H32,"P",101.325,G32)*1000</f>
+        <v>1763.1513779999998</v>
+      </c>
+      <c r="K32">
+        <f>[1]!Props("L","T",H32,"P",101.325,G32)*1000</f>
+        <v>0.12148516220000001</v>
+      </c>
+      <c r="L32">
+        <f>[1]!Props("V","T",H32,"P",101.325,G32)*1000</f>
+        <v>29.531534013677458</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>-80</v>
       </c>
@@ -901,23 +1448,46 @@
       <c r="F33">
         <v>155</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>36</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>193.14999999999998</v>
+      </c>
+      <c r="I33">
+        <f>[1]!Props("D","T",B33+273.15,"P",101.325,G33)</f>
+        <v>832.89109780000001</v>
+      </c>
+      <c r="J33">
+        <f>[1]!Props("C","T",H33,"P",101.325,G33)*1000</f>
+        <v>1676.9089779999999</v>
+      </c>
+      <c r="K33">
+        <f>[1]!Props("L","T",H33,"P",101.325,G33)*1000</f>
+        <v>0.12450940219999999</v>
+      </c>
+      <c r="L33">
+        <f>[1]!Props("V","T",H33,"P",101.325,G33)*1000</f>
+        <v>102.26265433491888</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -936,8 +1506,23 @@
       <c r="F39" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>1</v>
+      </c>
+      <c r="I39" t="s">
+        <v>2</v>
+      </c>
+      <c r="J39" t="s">
+        <v>3</v>
+      </c>
+      <c r="K39" t="s">
+        <v>4</v>
+      </c>
+      <c r="L39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -956,8 +1541,23 @@
       <c r="F40" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>28</v>
+      </c>
+      <c r="I40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" t="s">
+        <v>8</v>
+      </c>
+      <c r="K40" t="s">
+        <v>9</v>
+      </c>
+      <c r="L40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>-60</v>
       </c>
@@ -976,8 +1576,31 @@
       <c r="F41">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>35</v>
+      </c>
+      <c r="H41">
+        <f>B41+273.15</f>
+        <v>373.15</v>
+      </c>
+      <c r="I41">
+        <f>[1]!Props("D","T",B41+273.15,"P",101.325,G41)</f>
+        <v>1479.6373222499999</v>
+      </c>
+      <c r="J41">
+        <f>[1]!Props("C","T",H41,"P",101.325,G41)*1000</f>
+        <v>1192.2907422000001</v>
+      </c>
+      <c r="K41">
+        <f>[1]!Props("L","T",H41,"P",101.325,G41)*1000</f>
+        <v>6.8199979105000016E-2</v>
+      </c>
+      <c r="L41">
+        <f>[1]!Props("V","T",H41,"P",101.325,G41)*1000</f>
+        <v>0.56363729634069415</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>80</v>
       </c>
@@ -993,8 +1616,31 @@
       <c r="F42">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>35</v>
+      </c>
+      <c r="H42">
+        <f t="shared" ref="H42:H50" si="2">B42+273.15</f>
+        <v>353.15</v>
+      </c>
+      <c r="I42">
+        <f>[1]!Props("D","T",B42+273.15,"P",101.325,G42)</f>
+        <v>1498.0070222499999</v>
+      </c>
+      <c r="J42">
+        <f>[1]!Props("C","T",H42,"P",101.325,G42)*1000</f>
+        <v>1175.1149822</v>
+      </c>
+      <c r="K42">
+        <f>[1]!Props("L","T",H42,"P",101.325,G42)*1000</f>
+        <v>6.9866645105E-2</v>
+      </c>
+      <c r="L42">
+        <f>[1]!Props("V","T",H42,"P",101.325,G42)*1000</f>
+        <v>0.63681186338965257</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>60</v>
       </c>
@@ -1010,8 +1656,31 @@
       <c r="F43">
         <v>0.79</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>35</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="2"/>
+        <v>333.15</v>
+      </c>
+      <c r="I43">
+        <f>[1]!Props("D","T",B43+273.15,"P",101.325,G43)</f>
+        <v>1516.3767222499998</v>
+      </c>
+      <c r="J43">
+        <f>[1]!Props("C","T",H43,"P",101.325,G43)*1000</f>
+        <v>1157.9392221999999</v>
+      </c>
+      <c r="K43">
+        <f>[1]!Props("L","T",H43,"P",101.325,G43)*1000</f>
+        <v>7.1533311105000011E-2</v>
+      </c>
+      <c r="L43">
+        <f>[1]!Props("V","T",H43,"P",101.325,G43)*1000</f>
+        <v>0.72375733175798207</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>40</v>
       </c>
@@ -1027,8 +1696,31 @@
       <c r="F44">
         <v>0.87</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>35</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="2"/>
+        <v>313.14999999999998</v>
+      </c>
+      <c r="I44">
+        <f>[1]!Props("D","T",B44+273.15,"P",101.325,G44)</f>
+        <v>1534.74642225</v>
+      </c>
+      <c r="J44">
+        <f>[1]!Props("C","T",H44,"P",101.325,G44)*1000</f>
+        <v>1140.7634622</v>
+      </c>
+      <c r="K44">
+        <f>[1]!Props("L","T",H44,"P",101.325,G44)*1000</f>
+        <v>7.3199977105000008E-2</v>
+      </c>
+      <c r="L44">
+        <f>[1]!Props("V","T",H44,"P",101.325,G44)*1000</f>
+        <v>0.82745658290932989</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>20</v>
       </c>
@@ -1044,8 +1736,31 @@
       <c r="F45">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>35</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="2"/>
+        <v>293.14999999999998</v>
+      </c>
+      <c r="I45">
+        <f>[1]!Props("D","T",B45+273.15,"P",101.325,G45)</f>
+        <v>1553.11612225</v>
+      </c>
+      <c r="J45">
+        <f>[1]!Props("C","T",H45,"P",101.325,G45)*1000</f>
+        <v>1123.5877022</v>
+      </c>
+      <c r="K45">
+        <f>[1]!Props("L","T",H45,"P",101.325,G45)*1000</f>
+        <v>7.4866643105000005E-2</v>
+      </c>
+      <c r="L45">
+        <f>[1]!Props("V","T",H45,"P",101.325,G45)*1000</f>
+        <v>0.95162942647977644</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>0</v>
       </c>
@@ -1061,8 +1776,31 @@
       <c r="F46">
         <v>1.06</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>35</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="2"/>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="I46">
+        <f>[1]!Props("D","T",B46+273.15,"P",101.325,G46)</f>
+        <v>1571.48582225</v>
+      </c>
+      <c r="J46">
+        <f>[1]!Props("C","T",H46,"P",101.325,G46)*1000</f>
+        <v>1106.4119422000001</v>
+      </c>
+      <c r="K46">
+        <f>[1]!Props("L","T",H46,"P",101.325,G46)*1000</f>
+        <v>7.6533309105000016E-2</v>
+      </c>
+      <c r="L46">
+        <f>[1]!Props("V","T",H46,"P",101.325,G46)*1000</f>
+        <v>1.1009330737952496</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>-20</v>
       </c>
@@ -1078,8 +1816,31 @@
       <c r="F47">
         <v>1.21</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>35</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="2"/>
+        <v>253.14999999999998</v>
+      </c>
+      <c r="I47">
+        <f>[1]!Props("D","T",B47+273.15,"P",101.325,G47)</f>
+        <v>1589.8555222499999</v>
+      </c>
+      <c r="J47">
+        <f>[1]!Props("C","T",H47,"P",101.325,G47)*1000</f>
+        <v>1089.2361822</v>
+      </c>
+      <c r="K47">
+        <f>[1]!Props("L","T",H47,"P",101.325,G47)*1000</f>
+        <v>7.8199975105E-2</v>
+      </c>
+      <c r="L47">
+        <f>[1]!Props("V","T",H47,"P",101.325,G47)*1000</f>
+        <v>1.2812219873954174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>-40</v>
       </c>
@@ -1095,8 +1856,31 @@
       <c r="F48">
         <v>1.42</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>35</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="2"/>
+        <v>233.14999999999998</v>
+      </c>
+      <c r="I48">
+        <f>[1]!Props("D","T",B48+273.15,"P",101.325,G48)</f>
+        <v>1608.2252222499999</v>
+      </c>
+      <c r="J48">
+        <f>[1]!Props("C","T",H48,"P",101.325,G48)*1000</f>
+        <v>1072.0604221999999</v>
+      </c>
+      <c r="K48">
+        <f>[1]!Props("L","T",H48,"P",101.325,G48)*1000</f>
+        <v>7.9866641105000011E-2</v>
+      </c>
+      <c r="L48">
+        <f>[1]!Props("V","T",H48,"P",101.325,G48)*1000</f>
+        <v>1.4998860149528046</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>-60</v>
       </c>
@@ -1112,8 +1896,31 @@
       <c r="F49">
         <v>1.74</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>35</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="2"/>
+        <v>213.14999999999998</v>
+      </c>
+      <c r="I49">
+        <f>[1]!Props("D","T",B49+273.15,"P",101.325,G49)</f>
+        <v>1626.5949222499999</v>
+      </c>
+      <c r="J49">
+        <f>[1]!Props("C","T",H49,"P",101.325,G49)*1000</f>
+        <v>1054.8846621999999</v>
+      </c>
+      <c r="K49">
+        <f>[1]!Props("L","T",H49,"P",101.325,G49)*1000</f>
+        <v>8.1533307105000008E-2</v>
+      </c>
+      <c r="L49">
+        <f>[1]!Props("V","T",H49,"P",101.325,G49)*1000</f>
+        <v>1.7662921418018587</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>-80</v>
       </c>
@@ -1129,23 +1936,46 @@
       <c r="F50">
         <v>2.2400000000000002</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>35</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="2"/>
+        <v>193.14999999999998</v>
+      </c>
+      <c r="I50">
+        <f>[1]!Props("D","T",B50+273.15,"P",101.325,G50)</f>
+        <v>1644.9646222499998</v>
+      </c>
+      <c r="J50">
+        <f>[1]!Props("C","T",H50,"P",101.325,G50)*1000</f>
+        <v>1037.7089021999998</v>
+      </c>
+      <c r="K50">
+        <f>[1]!Props("L","T",H50,"P",101.325,G50)*1000</f>
+        <v>8.3199973105000005E-2</v>
+      </c>
+      <c r="L50">
+        <f>[1]!Props("V","T",H50,"P",101.325,G50)*1000</f>
+        <v>2.0923639372004286</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -1164,8 +1994,23 @@
       <c r="F56" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
+        <v>1</v>
+      </c>
+      <c r="I56" t="s">
+        <v>2</v>
+      </c>
+      <c r="J56" t="s">
+        <v>3</v>
+      </c>
+      <c r="K56" t="s">
+        <v>4</v>
+      </c>
+      <c r="L56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -1184,8 +2029,23 @@
       <c r="F57" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
+        <v>28</v>
+      </c>
+      <c r="I57" t="s">
+        <v>7</v>
+      </c>
+      <c r="J57" t="s">
+        <v>8</v>
+      </c>
+      <c r="K57" t="s">
+        <v>9</v>
+      </c>
+      <c r="L57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>-100</v>
       </c>
@@ -1204,8 +2064,31 @@
       <c r="F58">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>34</v>
+      </c>
+      <c r="H58">
+        <f>B58+273.15</f>
+        <v>373.15</v>
+      </c>
+      <c r="I58">
+        <f>[1]!Props("D","T",B58+273.15,"P",101.325,G58)</f>
+        <v>835.58212499999991</v>
+      </c>
+      <c r="J58">
+        <f>[1]!Props("C","T",H58,"P",101.325,G58)*1000</f>
+        <v>1777.5080355</v>
+      </c>
+      <c r="K58">
+        <f>[1]!Props("L","T",H58,"P",101.325,G58)*1000</f>
+        <v>0.10148908395</v>
+      </c>
+      <c r="L58">
+        <f>[1]!Props("V","T",H58,"P",101.325,G58)*1000</f>
+        <v>0.98714651104989293</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>80</v>
       </c>
@@ -1221,8 +2104,31 @@
       <c r="F59">
         <v>1.19</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>34</v>
+      </c>
+      <c r="H59">
+        <f t="shared" ref="H59:H67" si="3">B59+273.15</f>
+        <v>353.15</v>
+      </c>
+      <c r="I59">
+        <f>[1]!Props("D","T",B59+273.15,"P",101.325,G59)</f>
+        <v>853.63212499999997</v>
+      </c>
+      <c r="J59">
+        <f>[1]!Props("C","T",H59,"P",101.325,G59)*1000</f>
+        <v>1747.8246354999999</v>
+      </c>
+      <c r="K59">
+        <f>[1]!Props("L","T",H59,"P",101.325,G59)*1000</f>
+        <v>0.10717242395000001</v>
+      </c>
+      <c r="L59">
+        <f>[1]!Props("V","T",H59,"P",101.325,G59)*1000</f>
+        <v>1.1832239541272827</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>60</v>
       </c>
@@ -1238,8 +2144,31 @@
       <c r="F60">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60" t="s">
+        <v>34</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="3"/>
+        <v>333.15</v>
+      </c>
+      <c r="I60">
+        <f>[1]!Props("D","T",B60+273.15,"P",101.325,G60)</f>
+        <v>871.68212499999993</v>
+      </c>
+      <c r="J60">
+        <f>[1]!Props("C","T",H60,"P",101.325,G60)*1000</f>
+        <v>1718.1412354999998</v>
+      </c>
+      <c r="K60">
+        <f>[1]!Props("L","T",H60,"P",101.325,G60)*1000</f>
+        <v>0.11285576395000001</v>
+      </c>
+      <c r="L60">
+        <f>[1]!Props("V","T",H60,"P",101.325,G60)*1000</f>
+        <v>1.5061199956878544</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>40</v>
       </c>
@@ -1255,8 +2184,31 @@
       <c r="F61">
         <v>2.14</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>34</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="3"/>
+        <v>313.14999999999998</v>
+      </c>
+      <c r="I61">
+        <f>[1]!Props("D","T",B61+273.15,"P",101.325,G61)</f>
+        <v>889.73212499999988</v>
+      </c>
+      <c r="J61">
+        <f>[1]!Props("C","T",H61,"P",101.325,G61)*1000</f>
+        <v>1688.4578354999999</v>
+      </c>
+      <c r="K61">
+        <f>[1]!Props("L","T",H61,"P",101.325,G61)*1000</f>
+        <v>0.11853910395000002</v>
+      </c>
+      <c r="L61">
+        <f>[1]!Props("V","T",H61,"P",101.325,G61)*1000</f>
+        <v>2.03591423149288</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>20</v>
       </c>
@@ -1272,8 +2224,31 @@
       <c r="F62">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>34</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="3"/>
+        <v>293.14999999999998</v>
+      </c>
+      <c r="I62">
+        <f>[1]!Props("D","T",B62+273.15,"P",101.325,G62)</f>
+        <v>907.78212499999995</v>
+      </c>
+      <c r="J62">
+        <f>[1]!Props("C","T",H62,"P",101.325,G62)*1000</f>
+        <v>1658.7744354999998</v>
+      </c>
+      <c r="K62">
+        <f>[1]!Props("L","T",H62,"P",101.325,G62)*1000</f>
+        <v>0.12422244395</v>
+      </c>
+      <c r="L62">
+        <f>[1]!Props("V","T",H62,"P",101.325,G62)*1000</f>
+        <v>2.9225817278354334</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>0</v>
       </c>
@@ -1289,8 +2264,31 @@
       <c r="F63">
         <v>4.3499999999999996</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>34</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="3"/>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="I63">
+        <f>[1]!Props("D","T",B63+273.15,"P",101.325,G63)</f>
+        <v>925.83212499999991</v>
+      </c>
+      <c r="J63">
+        <f>[1]!Props("C","T",H63,"P",101.325,G63)*1000</f>
+        <v>1629.0910354999999</v>
+      </c>
+      <c r="K63">
+        <f>[1]!Props("L","T",H63,"P",101.325,G63)*1000</f>
+        <v>0.12990578395000002</v>
+      </c>
+      <c r="L63">
+        <f>[1]!Props("V","T",H63,"P",101.325,G63)*1000</f>
+        <v>4.4553428935727659</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>-20</v>
       </c>
@@ -1306,8 +2304,31 @@
       <c r="F64">
         <v>6.79</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
+        <v>34</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="3"/>
+        <v>253.14999999999998</v>
+      </c>
+      <c r="I64">
+        <f>[1]!Props("D","T",B64+273.15,"P",101.325,G64)</f>
+        <v>943.88212499999997</v>
+      </c>
+      <c r="J64">
+        <f>[1]!Props("C","T",H64,"P",101.325,G64)*1000</f>
+        <v>1599.4076355</v>
+      </c>
+      <c r="K64">
+        <f>[1]!Props("L","T",H64,"P",101.325,G64)*1000</f>
+        <v>0.13558912395</v>
+      </c>
+      <c r="L64">
+        <f>[1]!Props("V","T",H64,"P",101.325,G64)*1000</f>
+        <v>7.212783323967046</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>-40</v>
       </c>
@@ -1323,8 +2344,31 @@
       <c r="F65">
         <v>11.6</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
+        <v>34</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="3"/>
+        <v>233.14999999999998</v>
+      </c>
+      <c r="I65">
+        <f>[1]!Props("D","T",B65+273.15,"P",101.325,G65)</f>
+        <v>961.93212499999993</v>
+      </c>
+      <c r="J65">
+        <f>[1]!Props("C","T",H65,"P",101.325,G65)*1000</f>
+        <v>1569.7242354999998</v>
+      </c>
+      <c r="K65">
+        <f>[1]!Props("L","T",H65,"P",101.325,G65)*1000</f>
+        <v>0.14127246395000001</v>
+      </c>
+      <c r="L65">
+        <f>[1]!Props("V","T",H65,"P",101.325,G65)*1000</f>
+        <v>12.40029224669523</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>-60</v>
       </c>
@@ -1340,23 +2384,46 @@
       <c r="F66">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
+        <v>34</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="3"/>
+        <v>213.14999999999998</v>
+      </c>
+      <c r="I66">
+        <f>[1]!Props("D","T",B66+273.15,"P",101.325,G66)</f>
+        <v>979.98212499999988</v>
+      </c>
+      <c r="J66">
+        <f>[1]!Props("C","T",H66,"P",101.325,G66)*1000</f>
+        <v>1540.0408355</v>
+      </c>
+      <c r="K66">
+        <f>[1]!Props("L","T",H66,"P",101.325,G66)*1000</f>
+        <v>0.14695580395000002</v>
+      </c>
+      <c r="L66">
+        <f>[1]!Props("V","T",H66,"P",101.325,G66)*1000</f>
+        <v>22.639573341451023</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -1375,8 +2442,23 @@
       <c r="F72" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H72" t="s">
+        <v>1</v>
+      </c>
+      <c r="I72" t="s">
+        <v>2</v>
+      </c>
+      <c r="J72" t="s">
+        <v>3</v>
+      </c>
+      <c r="K72" t="s">
+        <v>4</v>
+      </c>
+      <c r="L72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -1395,8 +2477,23 @@
       <c r="F73" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H73" t="s">
+        <v>28</v>
+      </c>
+      <c r="I73" t="s">
+        <v>7</v>
+      </c>
+      <c r="J73" t="s">
+        <v>8</v>
+      </c>
+      <c r="K73" t="s">
+        <v>9</v>
+      </c>
+      <c r="L73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>-93</v>
       </c>
@@ -1415,8 +2512,31 @@
       <c r="F74">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>33</v>
+      </c>
+      <c r="H74">
+        <f>B74+273.15</f>
+        <v>373.15</v>
+      </c>
+      <c r="I74">
+        <f>[1]!Props("D","T",B74+273.15,"P",101.325,G74)</f>
+        <v>773.17765600000007</v>
+      </c>
+      <c r="J74">
+        <f>[1]!Props("C","T",H74,"P",101.325,G74)*1000</f>
+        <v>1940.1054220000001</v>
+      </c>
+      <c r="K74">
+        <f>[1]!Props("L","T",H74,"P",101.325,G74)*1000</f>
+        <v>9.3491242200000019E-2</v>
+      </c>
+      <c r="L74">
+        <f>[1]!Props("V","T",H74,"P",101.325,G74)*1000</f>
+        <v>0.53979794378338164</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>80</v>
       </c>
@@ -1432,8 +2552,31 @@
       <c r="F75">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
+        <v>33</v>
+      </c>
+      <c r="H75">
+        <f t="shared" ref="H75:H83" si="4">B75+273.15</f>
+        <v>353.15</v>
+      </c>
+      <c r="I75">
+        <f>[1]!Props("D","T",B75+273.15,"P",101.325,G75)</f>
+        <v>793.69285600000012</v>
+      </c>
+      <c r="J75">
+        <f>[1]!Props("C","T",H75,"P",101.325,G75)*1000</f>
+        <v>1897.9478219999999</v>
+      </c>
+      <c r="K75">
+        <f>[1]!Props("L","T",H75,"P",101.325,G75)*1000</f>
+        <v>9.7715482200000023E-2</v>
+      </c>
+      <c r="L75">
+        <f>[1]!Props("V","T",H75,"P",101.325,G75)*1000</f>
+        <v>0.61785037874653748</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>60</v>
       </c>
@@ -1449,8 +2592,31 @@
       <c r="F76">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
+        <v>33</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="4"/>
+        <v>333.15</v>
+      </c>
+      <c r="I76">
+        <f>[1]!Props("D","T",B76+273.15,"P",101.325,G76)</f>
+        <v>814.20805600000006</v>
+      </c>
+      <c r="J76">
+        <f>[1]!Props("C","T",H76,"P",101.325,G76)*1000</f>
+        <v>1855.7902220000001</v>
+      </c>
+      <c r="K76">
+        <f>[1]!Props("L","T",H76,"P",101.325,G76)*1000</f>
+        <v>0.10193972220000001</v>
+      </c>
+      <c r="L76">
+        <f>[1]!Props("V","T",H76,"P",101.325,G76)*1000</f>
+        <v>0.75453132413221491</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>40</v>
       </c>
@@ -1466,8 +2632,31 @@
       <c r="F77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77" t="s">
+        <v>33</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="4"/>
+        <v>313.14999999999998</v>
+      </c>
+      <c r="I77">
+        <f>[1]!Props("D","T",B77+273.15,"P",101.325,G77)</f>
+        <v>834.72325600000011</v>
+      </c>
+      <c r="J77">
+        <f>[1]!Props("C","T",H77,"P",101.325,G77)*1000</f>
+        <v>1813.6326220000001</v>
+      </c>
+      <c r="K77">
+        <f>[1]!Props("L","T",H77,"P",101.325,G77)*1000</f>
+        <v>0.10616396220000002</v>
+      </c>
+      <c r="L77">
+        <f>[1]!Props("V","T",H77,"P",101.325,G77)*1000</f>
+        <v>0.98313486191862776</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>20</v>
       </c>
@@ -1483,8 +2672,31 @@
       <c r="F78">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78" t="s">
+        <v>33</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="4"/>
+        <v>293.14999999999998</v>
+      </c>
+      <c r="I78">
+        <f>[1]!Props("D","T",B78+273.15,"P",101.325,G78)</f>
+        <v>855.23845600000004</v>
+      </c>
+      <c r="J78">
+        <f>[1]!Props("C","T",H78,"P",101.325,G78)*1000</f>
+        <v>1771.4750219999999</v>
+      </c>
+      <c r="K78">
+        <f>[1]!Props("L","T",H78,"P",101.325,G78)*1000</f>
+        <v>0.11038820220000002</v>
+      </c>
+      <c r="L78">
+        <f>[1]!Props("V","T",H78,"P",101.325,G78)*1000</f>
+        <v>1.3667553554593177</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>0</v>
       </c>
@@ -1500,8 +2712,31 @@
       <c r="F79">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79" t="s">
+        <v>33</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="4"/>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="I79">
+        <f>[1]!Props("D","T",B79+273.15,"P",101.325,G79)</f>
+        <v>875.75365600000009</v>
+      </c>
+      <c r="J79">
+        <f>[1]!Props("C","T",H79,"P",101.325,G79)*1000</f>
+        <v>1729.3174220000001</v>
+      </c>
+      <c r="K79">
+        <f>[1]!Props("L","T",H79,"P",101.325,G79)*1000</f>
+        <v>0.11461244220000001</v>
+      </c>
+      <c r="L79">
+        <f>[1]!Props("V","T",H79,"P",101.325,G79)*1000</f>
+        <v>2.0272641371432725</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>-20</v>
       </c>
@@ -1517,8 +2752,31 @@
       <c r="F80">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80" t="s">
+        <v>33</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="4"/>
+        <v>253.14999999999998</v>
+      </c>
+      <c r="I80">
+        <f>[1]!Props("D","T",B80+273.15,"P",101.325,G80)</f>
+        <v>896.26885600000003</v>
+      </c>
+      <c r="J80">
+        <f>[1]!Props("C","T",H80,"P",101.325,G80)*1000</f>
+        <v>1687.1598219999998</v>
+      </c>
+      <c r="K80">
+        <f>[1]!Props("L","T",H80,"P",101.325,G80)*1000</f>
+        <v>0.11883668220000002</v>
+      </c>
+      <c r="L80">
+        <f>[1]!Props("V","T",H80,"P",101.325,G80)*1000</f>
+        <v>3.2082762513971228</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>-40</v>
       </c>
@@ -1534,8 +2792,31 @@
       <c r="F81">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81" t="s">
+        <v>33</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="4"/>
+        <v>233.14999999999998</v>
+      </c>
+      <c r="I81">
+        <f>[1]!Props("D","T",B81+273.15,"P",101.325,G81)</f>
+        <v>916.78405600000008</v>
+      </c>
+      <c r="J81">
+        <f>[1]!Props("C","T",H81,"P",101.325,G81)*1000</f>
+        <v>1645.0022220000001</v>
+      </c>
+      <c r="K81">
+        <f>[1]!Props("L","T",H81,"P",101.325,G81)*1000</f>
+        <v>0.12306092220000002</v>
+      </c>
+      <c r="L81">
+        <f>[1]!Props("V","T",H81,"P",101.325,G81)*1000</f>
+        <v>5.4172021342475229</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>-60</v>
       </c>
@@ -1551,8 +2832,31 @@
       <c r="F82">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82" t="s">
+        <v>33</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="4"/>
+        <v>213.14999999999998</v>
+      </c>
+      <c r="I82">
+        <f>[1]!Props("D","T",B82+273.15,"P",101.325,G82)</f>
+        <v>937.29925600000013</v>
+      </c>
+      <c r="J82">
+        <f>[1]!Props("C","T",H82,"P",101.325,G82)*1000</f>
+        <v>1602.8446220000001</v>
+      </c>
+      <c r="K82">
+        <f>[1]!Props("L","T",H82,"P",101.325,G82)*1000</f>
+        <v>0.12728516220000002</v>
+      </c>
+      <c r="L82">
+        <f>[1]!Props("V","T",H82,"P",101.325,G82)*1000</f>
+        <v>9.759334210639155</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>-80</v>
       </c>
@@ -1568,23 +2872,46 @@
       <c r="F83">
         <v>20</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83" t="s">
+        <v>33</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="4"/>
+        <v>193.14999999999998</v>
+      </c>
+      <c r="I83">
+        <f>[1]!Props("D","T",B83+273.15,"P",101.325,G83)</f>
+        <v>957.81445600000006</v>
+      </c>
+      <c r="J83">
+        <f>[1]!Props("C","T",H83,"P",101.325,G83)*1000</f>
+        <v>1560.6870220000001</v>
+      </c>
+      <c r="K83">
+        <f>[1]!Props("L","T",H83,"P",101.325,G83)*1000</f>
+        <v>0.13150940220000001</v>
+      </c>
+      <c r="L83">
+        <f>[1]!Props("V","T",H83,"P",101.325,G83)*1000</f>
+        <v>18.758892997503484</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -1603,8 +2930,23 @@
       <c r="F89" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H89" t="s">
+        <v>1</v>
+      </c>
+      <c r="I89" t="s">
+        <v>2</v>
+      </c>
+      <c r="J89" t="s">
+        <v>3</v>
+      </c>
+      <c r="K89" t="s">
+        <v>4</v>
+      </c>
+      <c r="L89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -1623,8 +2965,23 @@
       <c r="F90" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H90" t="s">
+        <v>28</v>
+      </c>
+      <c r="I90" t="s">
+        <v>7</v>
+      </c>
+      <c r="J90" t="s">
+        <v>8</v>
+      </c>
+      <c r="K90" t="s">
+        <v>9</v>
+      </c>
+      <c r="L90" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>-60</v>
       </c>
@@ -1643,8 +3000,31 @@
       <c r="F91">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G91" t="s">
+        <v>32</v>
+      </c>
+      <c r="H91">
+        <f>B91+273.15</f>
+        <v>373.15</v>
+      </c>
+      <c r="I91">
+        <f>[1]!Props("D","T",B91+273.15,"P",101.325,G91)</f>
+        <v>803.19795894999993</v>
+      </c>
+      <c r="J91">
+        <f>[1]!Props("C","T",H91,"P",101.325,G91)*1000</f>
+        <v>1926.8854105</v>
+      </c>
+      <c r="K91">
+        <f>[1]!Props("L","T",H91,"P",101.325,G91)*1000</f>
+        <v>0.11073295895</v>
+      </c>
+      <c r="L91">
+        <f>[1]!Props("V","T",H91,"P",101.325,G91)*1000</f>
+        <v>0.41531214384547482</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>80</v>
       </c>
@@ -1660,8 +3040,31 @@
       <c r="F92">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92" t="s">
+        <v>32</v>
+      </c>
+      <c r="H92">
+        <f t="shared" ref="H92:H100" si="5">B92+273.15</f>
+        <v>353.15</v>
+      </c>
+      <c r="I92">
+        <f>[1]!Props("D","T",B92+273.15,"P",101.325,G92)</f>
+        <v>819.23129894999988</v>
+      </c>
+      <c r="J92">
+        <f>[1]!Props("C","T",H92,"P",101.325,G92)*1000</f>
+        <v>1896.5520105000001</v>
+      </c>
+      <c r="K92">
+        <f>[1]!Props("L","T",H92,"P",101.325,G92)*1000</f>
+        <v>0.11596629895</v>
+      </c>
+      <c r="L92">
+        <f>[1]!Props("V","T",H92,"P",101.325,G92)*1000</f>
+        <v>0.4571198797165722</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>60</v>
       </c>
@@ -1677,8 +3080,31 @@
       <c r="F93">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93" t="s">
+        <v>32</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="5"/>
+        <v>333.15</v>
+      </c>
+      <c r="I93">
+        <f>[1]!Props("D","T",B93+273.15,"P",101.325,G93)</f>
+        <v>835.26463894999995</v>
+      </c>
+      <c r="J93">
+        <f>[1]!Props("C","T",H93,"P",101.325,G93)*1000</f>
+        <v>1866.2186105000001</v>
+      </c>
+      <c r="K93">
+        <f>[1]!Props("L","T",H93,"P",101.325,G93)*1000</f>
+        <v>0.12119963894999999</v>
+      </c>
+      <c r="L93">
+        <f>[1]!Props("V","T",H93,"P",101.325,G93)*1000</f>
+        <v>0.53856799678503908</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>40</v>
       </c>
@@ -1694,8 +3120,31 @@
       <c r="F94">
         <v>0.72</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94" t="s">
+        <v>32</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="5"/>
+        <v>313.14999999999998</v>
+      </c>
+      <c r="I94">
+        <f>[1]!Props("D","T",B94+273.15,"P",101.325,G94)</f>
+        <v>851.2979789499999</v>
+      </c>
+      <c r="J94">
+        <f>[1]!Props("C","T",H94,"P",101.325,G94)*1000</f>
+        <v>1835.8852105000001</v>
+      </c>
+      <c r="K94">
+        <f>[1]!Props("L","T",H94,"P",101.325,G94)*1000</f>
+        <v>0.12643297895</v>
+      </c>
+      <c r="L94">
+        <f>[1]!Props("V","T",H94,"P",101.325,G94)*1000</f>
+        <v>0.67921291059547484</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>20</v>
       </c>
@@ -1711,8 +3160,31 @@
       <c r="F95">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G95" t="s">
+        <v>32</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="5"/>
+        <v>293.14999999999998</v>
+      </c>
+      <c r="I95">
+        <f>[1]!Props("D","T",B95+273.15,"P",101.325,G95)</f>
+        <v>867.33131894999997</v>
+      </c>
+      <c r="J95">
+        <f>[1]!Props("C","T",H95,"P",101.325,G95)*1000</f>
+        <v>1805.5518104999999</v>
+      </c>
+      <c r="K95">
+        <f>[1]!Props("L","T",H95,"P",101.325,G95)*1000</f>
+        <v>0.13166631895</v>
+      </c>
+      <c r="L95">
+        <f>[1]!Props("V","T",H95,"P",101.325,G95)*1000</f>
+        <v>0.9169090886268797</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>0</v>
       </c>
@@ -1728,8 +3200,31 @@
       <c r="F96">
         <v>1.24</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96" t="s">
+        <v>32</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="5"/>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="I96">
+        <f>[1]!Props("D","T",B96+273.15,"P",101.325,G96)</f>
+        <v>883.36465894999992</v>
+      </c>
+      <c r="J96">
+        <f>[1]!Props("C","T",H96,"P",101.325,G96)*1000</f>
+        <v>1775.2184104999999</v>
+      </c>
+      <c r="K96">
+        <f>[1]!Props("L","T",H96,"P",101.325,G96)*1000</f>
+        <v>0.13689965894999997</v>
+      </c>
+      <c r="L96">
+        <f>[1]!Props("V","T",H96,"P",101.325,G96)*1000</f>
+        <v>1.3249563723491296</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>-20</v>
       </c>
@@ -1745,8 +3240,31 @@
       <c r="F97">
         <v>1.89</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G97" t="s">
+        <v>32</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="5"/>
+        <v>253.14999999999998</v>
+      </c>
+      <c r="I97">
+        <f>[1]!Props("D","T",B97+273.15,"P",101.325,G97)</f>
+        <v>899.39799894999999</v>
+      </c>
+      <c r="J97">
+        <f>[1]!Props("C","T",H97,"P",101.325,G97)*1000</f>
+        <v>1744.8850104999999</v>
+      </c>
+      <c r="K97">
+        <f>[1]!Props("L","T",H97,"P",101.325,G97)*1000</f>
+        <v>0.14213299895000001</v>
+      </c>
+      <c r="L97">
+        <f>[1]!Props("V","T",H97,"P",101.325,G97)*1000</f>
+        <v>2.0494240785085527</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>-40</v>
       </c>
@@ -1762,8 +3280,31 @@
       <c r="F98">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G98" t="s">
+        <v>32</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="5"/>
+        <v>233.14999999999998</v>
+      </c>
+      <c r="I98">
+        <f>[1]!Props("D","T",B98+273.15,"P",101.325,G98)</f>
+        <v>915.43133894999994</v>
+      </c>
+      <c r="J98">
+        <f>[1]!Props("C","T",H98,"P",101.325,G98)*1000</f>
+        <v>1714.5516105000002</v>
+      </c>
+      <c r="K98">
+        <f>[1]!Props("L","T",H98,"P",101.325,G98)*1000</f>
+        <v>0.14736633895000001</v>
+      </c>
+      <c r="L98">
+        <f>[1]!Props("V","T",H98,"P",101.325,G98)*1000</f>
+        <v>3.3932592845256249</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>-60</v>
       </c>
@@ -1779,23 +3320,46 @@
       <c r="F99">
         <v>6.61</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G99" t="s">
+        <v>32</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="5"/>
+        <v>213.14999999999998</v>
+      </c>
+      <c r="I99">
+        <f>[1]!Props("D","T",B99+273.15,"P",101.325,G99)</f>
+        <v>931.46467894999989</v>
+      </c>
+      <c r="J99">
+        <f>[1]!Props("C","T",H99,"P",101.325,G99)*1000</f>
+        <v>1684.2182105000002</v>
+      </c>
+      <c r="K99">
+        <f>[1]!Props("L","T",H99,"P",101.325,G99)*1000</f>
+        <v>0.15259967894999998</v>
+      </c>
+      <c r="L99">
+        <f>[1]!Props("V","T",H99,"P",101.325,G99)*1000</f>
+        <v>6.0139139992169257</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>0</v>
       </c>
@@ -1814,8 +3378,23 @@
       <c r="F105" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H105" t="s">
+        <v>1</v>
+      </c>
+      <c r="I105" t="s">
+        <v>2</v>
+      </c>
+      <c r="J105" t="s">
+        <v>3</v>
+      </c>
+      <c r="K105" t="s">
+        <v>4</v>
+      </c>
+      <c r="L105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>6</v>
       </c>
@@ -1834,8 +3413,23 @@
       <c r="F106" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H106" t="s">
+        <v>28</v>
+      </c>
+      <c r="I106" t="s">
+        <v>7</v>
+      </c>
+      <c r="J106" t="s">
+        <v>8</v>
+      </c>
+      <c r="K106" t="s">
+        <v>9</v>
+      </c>
+      <c r="L106" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>-60</v>
       </c>
@@ -1854,8 +3448,31 @@
       <c r="F107">
         <v>0.77500000000000002</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G107" t="s">
+        <v>31</v>
+      </c>
+      <c r="H107">
+        <f>B107+273.15</f>
+        <v>333.15</v>
+      </c>
+      <c r="I107">
+        <f>[1]!Props("D","T",B107+273.15,"P",101.325,G107)</f>
+        <v>814.58020439999996</v>
+      </c>
+      <c r="J107">
+        <f>[1]!Props("C","T",H107,"P",101.325,G107)*1000</f>
+        <v>1937.3325439999999</v>
+      </c>
+      <c r="K107">
+        <f>[1]!Props("L","T",H107,"P",101.325,G107)*1000</f>
+        <v>0.12366642650000001</v>
+      </c>
+      <c r="L107">
+        <f>[1]!Props("V","T",H107,"P",101.325,G107)*1000</f>
+        <v>0.82997037896038439</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B108">
         <v>40</v>
       </c>
@@ -1871,8 +3488,31 @@
       <c r="F108">
         <v>0.89500000000000002</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G108" t="s">
+        <v>31</v>
+      </c>
+      <c r="H108">
+        <f t="shared" ref="H108:H116" si="6">B108+273.15</f>
+        <v>313.14999999999998</v>
+      </c>
+      <c r="I108">
+        <f>[1]!Props("D","T",B108+273.15,"P",101.325,G108)</f>
+        <v>830.02068439999994</v>
+      </c>
+      <c r="J108">
+        <f>[1]!Props("C","T",H108,"P",101.325,G108)*1000</f>
+        <v>1866.7373439999999</v>
+      </c>
+      <c r="K108">
+        <f>[1]!Props("L","T",H108,"P",101.325,G108)*1000</f>
+        <v>0.12844022650000003</v>
+      </c>
+      <c r="L108">
+        <f>[1]!Props("V","T",H108,"P",101.325,G108)*1000</f>
+        <v>0.8623202385875085</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>20</v>
       </c>
@@ -1888,8 +3528,31 @@
       <c r="F109">
         <v>1.069</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G109" t="s">
+        <v>31</v>
+      </c>
+      <c r="H109">
+        <f t="shared" si="6"/>
+        <v>293.14999999999998</v>
+      </c>
+      <c r="I109">
+        <f>[1]!Props("D","T",B109+273.15,"P",101.325,G109)</f>
+        <v>845.46116440000003</v>
+      </c>
+      <c r="J109">
+        <f>[1]!Props("C","T",H109,"P",101.325,G109)*1000</f>
+        <v>1796.1421439999999</v>
+      </c>
+      <c r="K109">
+        <f>[1]!Props("L","T",H109,"P",101.325,G109)*1000</f>
+        <v>0.13321402650000003</v>
+      </c>
+      <c r="L109">
+        <f>[1]!Props("V","T",H109,"P",101.325,G109)*1000</f>
+        <v>0.99460592571877182</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B110">
         <v>0</v>
       </c>
@@ -1905,8 +3568,31 @@
       <c r="F110">
         <v>1.3360000000000001</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G110" t="s">
+        <v>31</v>
+      </c>
+      <c r="H110">
+        <f t="shared" si="6"/>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="I110">
+        <f>[1]!Props("D","T",B110+273.15,"P",101.325,G110)</f>
+        <v>860.90164440000001</v>
+      </c>
+      <c r="J110">
+        <f>[1]!Props("C","T",H110,"P",101.325,G110)*1000</f>
+        <v>1725.5469439999999</v>
+      </c>
+      <c r="K110">
+        <f>[1]!Props("L","T",H110,"P",101.325,G110)*1000</f>
+        <v>0.13798782650000002</v>
+      </c>
+      <c r="L110">
+        <f>[1]!Props("V","T",H110,"P",101.325,G110)*1000</f>
+        <v>1.2735323546142157</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B111">
         <v>-20</v>
       </c>
@@ -1922,8 +3608,31 @@
       <c r="F111">
         <v>1.784</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G111" t="s">
+        <v>31</v>
+      </c>
+      <c r="H111">
+        <f t="shared" si="6"/>
+        <v>253.14999999999998</v>
+      </c>
+      <c r="I111">
+        <f>[1]!Props("D","T",B111+273.15,"P",101.325,G111)</f>
+        <v>876.34212439999999</v>
+      </c>
+      <c r="J111">
+        <f>[1]!Props("C","T",H111,"P",101.325,G111)*1000</f>
+        <v>1654.951744</v>
+      </c>
+      <c r="K111">
+        <f>[1]!Props("L","T",H111,"P",101.325,G111)*1000</f>
+        <v>0.14276162649999999</v>
+      </c>
+      <c r="L111">
+        <f>[1]!Props("V","T",H111,"P",101.325,G111)*1000</f>
+        <v>1.810278529557257</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B112">
         <v>-40</v>
       </c>
@@ -1939,8 +3648,31 @@
       <c r="F112">
         <v>2.6339999999999999</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G112" t="s">
+        <v>31</v>
+      </c>
+      <c r="H112">
+        <f t="shared" si="6"/>
+        <v>233.14999999999998</v>
+      </c>
+      <c r="I112">
+        <f>[1]!Props("D","T",B112+273.15,"P",101.325,G112)</f>
+        <v>891.78260439999997</v>
+      </c>
+      <c r="J112">
+        <f>[1]!Props("C","T",H112,"P",101.325,G112)*1000</f>
+        <v>1584.3565439999998</v>
+      </c>
+      <c r="K112">
+        <f>[1]!Props("L","T",H112,"P",101.325,G112)*1000</f>
+        <v>0.14753542650000001</v>
+      </c>
+      <c r="L112">
+        <f>[1]!Props("V","T",H112,"P",101.325,G112)*1000</f>
+        <v>2.8566517241410465</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B113">
         <v>-60</v>
       </c>
@@ -1956,8 +3688,31 @@
       <c r="F113">
         <v>4.5810000000000004</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G113" t="s">
+        <v>31</v>
+      </c>
+      <c r="H113">
+        <f t="shared" si="6"/>
+        <v>213.14999999999998</v>
+      </c>
+      <c r="I113">
+        <f>[1]!Props("D","T",B113+273.15,"P",101.325,G113)</f>
+        <v>907.22308439999995</v>
+      </c>
+      <c r="J113">
+        <f>[1]!Props("C","T",H113,"P",101.325,G113)*1000</f>
+        <v>1513.761344</v>
+      </c>
+      <c r="K113">
+        <f>[1]!Props("L","T",H113,"P",101.325,G113)*1000</f>
+        <v>0.15230922650000001</v>
+      </c>
+      <c r="L113">
+        <f>[1]!Props("V","T",H113,"P",101.325,G113)*1000</f>
+        <v>5.0043268547780393</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B114">
         <v>-80</v>
       </c>
@@ -1973,23 +3728,46 @@
       <c r="F114">
         <v>10.71</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G114" t="s">
+        <v>31</v>
+      </c>
+      <c r="H114">
+        <f t="shared" si="6"/>
+        <v>193.14999999999998</v>
+      </c>
+      <c r="I114">
+        <f>[1]!Props("D","T",B114+273.15,"P",101.325,G114)</f>
+        <v>922.66356439999993</v>
+      </c>
+      <c r="J114">
+        <f>[1]!Props("C","T",H114,"P",101.325,G114)*1000</f>
+        <v>1443.1661439999998</v>
+      </c>
+      <c r="K114">
+        <f>[1]!Props("L","T",H114,"P",101.325,G114)*1000</f>
+        <v>0.1570830265</v>
+      </c>
+      <c r="L114">
+        <f>[1]!Props("V","T",H114,"P",101.325,G114)*1000</f>
+        <v>9.7321886104290432</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>0</v>
       </c>
@@ -2008,8 +3786,23 @@
       <c r="F120" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H120" t="s">
+        <v>1</v>
+      </c>
+      <c r="I120" t="s">
+        <v>2</v>
+      </c>
+      <c r="J120" t="s">
+        <v>3</v>
+      </c>
+      <c r="K120" t="s">
+        <v>4</v>
+      </c>
+      <c r="L120" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>6</v>
       </c>
@@ -2028,8 +3821,23 @@
       <c r="F121" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H121" t="s">
+        <v>28</v>
+      </c>
+      <c r="I121" t="s">
+        <v>7</v>
+      </c>
+      <c r="J121" t="s">
+        <v>8</v>
+      </c>
+      <c r="K121" t="s">
+        <v>9</v>
+      </c>
+      <c r="L121" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>-96.7</v>
       </c>
@@ -2048,8 +3856,31 @@
       <c r="F122">
         <v>0.66</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G122" t="s">
+        <v>30</v>
+      </c>
+      <c r="H122">
+        <f>B122+273.15</f>
+        <v>373.15</v>
+      </c>
+      <c r="I122">
+        <f>[1]!Props("D","T",B122+273.15,"P",101.325,G122)</f>
+        <v>780.64735710000002</v>
+      </c>
+      <c r="J122">
+        <f>[1]!Props("C","T",H122,"P",101.325,G122)*1000</f>
+        <v>2170.0880849999999</v>
+      </c>
+      <c r="K122">
+        <f>[1]!Props("L","T",H122,"P",101.325,G122)*1000</f>
+        <v>0.10510384619999999</v>
+      </c>
+      <c r="L122">
+        <f>[1]!Props("V","T",H122,"P",101.325,G122)*1000</f>
+        <v>0.66566942723194344</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B123">
         <v>75</v>
       </c>
@@ -2065,8 +3896,31 @@
       <c r="F123">
         <v>0.86</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G123" t="s">
+        <v>30</v>
+      </c>
+      <c r="H123">
+        <f t="shared" ref="H123:H131" si="7">B123+273.15</f>
+        <v>348.15</v>
+      </c>
+      <c r="I123">
+        <f>[1]!Props("D","T",B123+273.15,"P",101.325,G123)</f>
+        <v>800.10150709999994</v>
+      </c>
+      <c r="J123">
+        <f>[1]!Props("C","T",H123,"P",101.325,G123)*1000</f>
+        <v>2039.6905849999998</v>
+      </c>
+      <c r="K123">
+        <f>[1]!Props("L","T",H123,"P",101.325,G123)*1000</f>
+        <v>0.10973014619999999</v>
+      </c>
+      <c r="L123">
+        <f>[1]!Props("V","T",H123,"P",101.325,G123)*1000</f>
+        <v>0.85218030826469426</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B124">
         <v>50</v>
       </c>
@@ -2082,8 +3936,31 @@
       <c r="F124">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G124" t="s">
+        <v>30</v>
+      </c>
+      <c r="H124">
+        <f t="shared" si="7"/>
+        <v>323.14999999999998</v>
+      </c>
+      <c r="I124">
+        <f>[1]!Props("D","T",B124+273.15,"P",101.325,G124)</f>
+        <v>819.55565709999996</v>
+      </c>
+      <c r="J124">
+        <f>[1]!Props("C","T",H124,"P",101.325,G124)*1000</f>
+        <v>1909.2930849999998</v>
+      </c>
+      <c r="K124">
+        <f>[1]!Props("L","T",H124,"P",101.325,G124)*1000</f>
+        <v>0.11435644619999999</v>
+      </c>
+      <c r="L124">
+        <f>[1]!Props("V","T",H124,"P",101.325,G124)*1000</f>
+        <v>1.0925057071670397</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B125">
         <v>25</v>
       </c>
@@ -2099,8 +3976,31 @@
       <c r="F125">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G125" t="s">
+        <v>30</v>
+      </c>
+      <c r="H125">
+        <f t="shared" si="7"/>
+        <v>298.14999999999998</v>
+      </c>
+      <c r="I125">
+        <f>[1]!Props("D","T",B125+273.15,"P",101.325,G125)</f>
+        <v>839.00980709999999</v>
+      </c>
+      <c r="J125">
+        <f>[1]!Props("C","T",H125,"P",101.325,G125)*1000</f>
+        <v>1778.895585</v>
+      </c>
+      <c r="K125">
+        <f>[1]!Props("L","T",H125,"P",101.325,G125)*1000</f>
+        <v>0.11898274619999999</v>
+      </c>
+      <c r="L125">
+        <f>[1]!Props("V","T",H125,"P",101.325,G125)*1000</f>
+        <v>1.4026046382022312</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B126">
         <v>0</v>
       </c>
@@ -2116,8 +4016,31 @@
       <c r="F126">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G126" t="s">
+        <v>30</v>
+      </c>
+      <c r="H126">
+        <f t="shared" si="7"/>
+        <v>273.14999999999998</v>
+      </c>
+      <c r="I126">
+        <f>[1]!Props("D","T",B126+273.15,"P",101.325,G126)</f>
+        <v>858.46395710000002</v>
+      </c>
+      <c r="J126">
+        <f>[1]!Props("C","T",H126,"P",101.325,G126)*1000</f>
+        <v>1648.4980849999999</v>
+      </c>
+      <c r="K126">
+        <f>[1]!Props("L","T",H126,"P",101.325,G126)*1000</f>
+        <v>0.12360904619999999</v>
+      </c>
+      <c r="L126">
+        <f>[1]!Props("V","T",H126,"P",101.325,G126)*1000</f>
+        <v>1.8032924465230089</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B127">
         <v>-25</v>
       </c>
@@ -2133,8 +4056,31 @@
       <c r="F127">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G127" t="s">
+        <v>30</v>
+      </c>
+      <c r="H127">
+        <f t="shared" si="7"/>
+        <v>248.14999999999998</v>
+      </c>
+      <c r="I127">
+        <f>[1]!Props("D","T",B127+273.15,"P",101.325,G127)</f>
+        <v>877.91810710000004</v>
+      </c>
+      <c r="J127">
+        <f>[1]!Props("C","T",H127,"P",101.325,G127)*1000</f>
+        <v>1518.1005849999997</v>
+      </c>
+      <c r="K127">
+        <f>[1]!Props("L","T",H127,"P",101.325,G127)*1000</f>
+        <v>0.12823534619999999</v>
+      </c>
+      <c r="L127">
+        <f>[1]!Props("V","T",H127,"P",101.325,G127)*1000</f>
+        <v>2.3217550182393718</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B128">
         <v>-50</v>
       </c>
@@ -2150,8 +4096,31 @@
       <c r="F128">
         <v>3</v>
       </c>
-    </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G128" t="s">
+        <v>30</v>
+      </c>
+      <c r="H128">
+        <f t="shared" si="7"/>
+        <v>223.14999999999998</v>
+      </c>
+      <c r="I128">
+        <f>[1]!Props("D","T",B128+273.15,"P",101.325,G128)</f>
+        <v>897.37225709999996</v>
+      </c>
+      <c r="J128">
+        <f>[1]!Props("C","T",H128,"P",101.325,G128)*1000</f>
+        <v>1387.7030849999999</v>
+      </c>
+      <c r="K128">
+        <f>[1]!Props("L","T",H128,"P",101.325,G128)*1000</f>
+        <v>0.13286164619999999</v>
+      </c>
+      <c r="L128">
+        <f>[1]!Props("V","T",H128,"P",101.325,G128)*1000</f>
+        <v>2.9935461563606656</v>
+      </c>
+    </row>
+    <row r="129" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B129">
         <v>-73</v>
       </c>
@@ -2166,6 +4135,29 @@
       </c>
       <c r="F129">
         <v>3.8</v>
+      </c>
+      <c r="G129" t="s">
+        <v>30</v>
+      </c>
+      <c r="H129">
+        <f t="shared" si="7"/>
+        <v>200.14999999999998</v>
+      </c>
+      <c r="I129">
+        <f>[1]!Props("D","T",B129+273.15,"P",101.325,G129)</f>
+        <v>915.27007509999999</v>
+      </c>
+      <c r="J129">
+        <f>[1]!Props("C","T",H129,"P",101.325,G129)*1000</f>
+        <v>1267.7373849999997</v>
+      </c>
+      <c r="K129">
+        <f>[1]!Props("L","T",H129,"P",101.325,G129)*1000</f>
+        <v>0.13711784220000001</v>
+      </c>
+      <c r="L129">
+        <f>[1]!Props("V","T",H129,"P",101.325,G129)*1000</f>
+        <v>3.7868051348243341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>